<commit_message>
Modified duplicates removed spreadsheet and added a new spreadsheet with all samples hand-coded.
</commit_message>
<xml_diff>
--- a/data/samples/data_duplicates_removed_samples.xlsx
+++ b/data/samples/data_duplicates_removed_samples.xlsx
@@ -1,28 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10319"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nish\projects\titleix\data\samples\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Becky/Desktop/DOE:OCR papers/samples/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{933B1F25-E01F-4AC2-99D9-D226B5F79F99}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C16BA4DD-315A-B442-ABC4-E70E7066C9C1}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="900" yWindow="3180" windowWidth="28800" windowHeight="12220" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="sample1" sheetId="1" r:id="rId1"/>
     <sheet name="sample2" sheetId="2" r:id="rId2"/>
     <sheet name="sample3" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet1" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="262">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="263">
   <si>
     <t>doc.comment_body</t>
   </si>
@@ -808,15 +809,25 @@
   </si>
   <si>
     <t>Please withdraw the regulation that appears at 34 CFR Part 99 which was effective Jan 2012 and which greatly diminished the privacy protections of FERPA Prove to us that our children are nothing but data sources to be mined by government and corporations Do what is right Sincerely Annette Kocka</t>
+  </si>
+  <si>
+    <t>Health &amp; Safety</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -871,15 +882,19 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1182,21 +1197,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C96"/>
+  <dimension ref="A1:D96"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="A9" sqref="A1:XFD1048576"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="8.85546875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="136.140625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="15.5703125" style="1" customWidth="1"/>
-    <col min="4" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="8.83203125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="136.1640625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="15.5" style="1" customWidth="1"/>
+    <col min="4" max="4" width="14.1640625" style="1" customWidth="1"/>
+    <col min="5" max="16384" width="9.1640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="2"/>
       <c r="B1" s="3" t="s">
         <v>0</v>
@@ -1204,8 +1220,11 @@
       <c r="C1" s="3" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="D1" s="5" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A2" s="3">
         <v>592</v>
       </c>
@@ -1216,7 +1235,7 @@
         <v>-0.1208333333</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="63" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" ht="64" x14ac:dyDescent="0.2">
       <c r="A3" s="3">
         <v>28</v>
       </c>
@@ -1227,7 +1246,7 @@
         <v>-9.4421487600000006E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="63" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" ht="64" x14ac:dyDescent="0.2">
       <c r="A4" s="3">
         <v>1720</v>
       </c>
@@ -1238,7 +1257,7 @@
         <v>-8.4932659899999999E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="63" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" ht="64" x14ac:dyDescent="0.2">
       <c r="A5" s="3">
         <v>626</v>
       </c>
@@ -1249,7 +1268,7 @@
         <v>-7.4999999999999997E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="78.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" ht="64" x14ac:dyDescent="0.2">
       <c r="A6" s="3">
         <v>1865</v>
       </c>
@@ -1260,7 +1279,7 @@
         <v>-5.4166666699999998E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="126" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" ht="112" x14ac:dyDescent="0.2">
       <c r="A7" s="3">
         <v>1049</v>
       </c>
@@ -1271,7 +1290,7 @@
         <v>-5.1431523E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A8" s="3">
         <v>2200</v>
       </c>
@@ -1282,7 +1301,7 @@
         <v>-0.05</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="94.5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" ht="80" x14ac:dyDescent="0.2">
       <c r="A9" s="3">
         <v>218</v>
       </c>
@@ -1293,7 +1312,7 @@
         <v>-6.5000000000000006E-3</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" s="3">
         <v>2593</v>
       </c>
@@ -1304,7 +1323,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" s="3">
         <v>1795</v>
       </c>
@@ -1315,7 +1334,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" s="3">
         <v>2308</v>
       </c>
@@ -1326,7 +1345,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="220.5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" ht="208" x14ac:dyDescent="0.2">
       <c r="A13" s="3">
         <v>149</v>
       </c>
@@ -1337,7 +1356,7 @@
         <v>7.5410700000000004E-3</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" ht="48" x14ac:dyDescent="0.2">
       <c r="A14" s="3">
         <v>2288</v>
       </c>
@@ -1348,7 +1367,7 @@
         <v>2.32142857E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="63" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" ht="48" x14ac:dyDescent="0.2">
       <c r="A15" s="3">
         <v>2399</v>
       </c>
@@ -1359,7 +1378,7 @@
         <v>5.3571428600000012E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="94.5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" ht="80" x14ac:dyDescent="0.2">
       <c r="A16" s="3">
         <v>2212</v>
       </c>
@@ -1370,7 +1389,7 @@
         <v>6.5000000000000002E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="78.75" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" ht="64" x14ac:dyDescent="0.2">
       <c r="A17" s="3">
         <v>605</v>
       </c>
@@ -1381,7 +1400,7 @@
         <v>7.0000000000000007E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="126" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" ht="112" x14ac:dyDescent="0.2">
       <c r="A18" s="3">
         <v>2293</v>
       </c>
@@ -1392,7 +1411,7 @@
         <v>7.03125E-2</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="189" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" ht="176" x14ac:dyDescent="0.2">
       <c r="A19" s="3">
         <v>710</v>
       </c>
@@ -1403,7 +1422,7 @@
         <v>8.8725490200000007E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A20" s="3">
         <v>2071</v>
       </c>
@@ -1414,7 +1433,7 @@
         <v>8.8732816500000006E-2</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="78.75" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" ht="64" x14ac:dyDescent="0.2">
       <c r="A21" s="3">
         <v>1137</v>
       </c>
@@ -1425,7 +1444,7 @@
         <v>8.8888888900000004E-2</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A22" s="3">
         <v>2198</v>
       </c>
@@ -1436,7 +1455,7 @@
         <v>9.6679760599999998E-2</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="126" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" ht="112" x14ac:dyDescent="0.2">
       <c r="A23" s="3">
         <v>2166</v>
       </c>
@@ -1447,7 +1466,7 @@
         <v>9.7619047600000008E-2</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="252" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" ht="224" x14ac:dyDescent="0.2">
       <c r="A24" s="3">
         <v>2418</v>
       </c>
@@ -1458,7 +1477,7 @@
         <v>9.8051948100000008E-2</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="63" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" ht="48" x14ac:dyDescent="0.2">
       <c r="A25" s="3">
         <v>1765</v>
       </c>
@@ -1469,7 +1488,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="94.5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" ht="80" x14ac:dyDescent="0.2">
       <c r="A26" s="3">
         <v>850</v>
       </c>
@@ -1480,7 +1499,7 @@
         <v>0.10166666670000001</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="94.5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" ht="96" x14ac:dyDescent="0.2">
       <c r="A27" s="3">
         <v>645</v>
       </c>
@@ -1491,7 +1510,7 @@
         <v>0.10625</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="173.25" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" ht="160" x14ac:dyDescent="0.2">
       <c r="A28" s="3">
         <v>2808</v>
       </c>
@@ -1502,7 +1521,7 @@
         <v>0.1084209441</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="63" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" ht="64" x14ac:dyDescent="0.2">
       <c r="A29" s="3">
         <v>1566</v>
       </c>
@@ -1513,7 +1532,7 @@
         <v>0.10909090909999999</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="220.5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" ht="192" x14ac:dyDescent="0.2">
       <c r="A30" s="3">
         <v>1937</v>
       </c>
@@ -1524,7 +1543,7 @@
         <v>0.11387755099999999</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" ht="48" x14ac:dyDescent="0.2">
       <c r="A31" s="3">
         <v>106</v>
       </c>
@@ -1535,7 +1554,7 @@
         <v>0.11428571429999999</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="78.75" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" ht="80" x14ac:dyDescent="0.2">
       <c r="A32" s="3">
         <v>775</v>
       </c>
@@ -1546,7 +1565,7 @@
         <v>0.1183333333</v>
       </c>
     </row>
-    <row r="33" spans="1:3" ht="267.75" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" ht="240" x14ac:dyDescent="0.2">
       <c r="A33" s="3">
         <v>1102</v>
       </c>
@@ -1557,7 +1576,7 @@
         <v>0.11881720430000001</v>
       </c>
     </row>
-    <row r="34" spans="1:3" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A34" s="3">
         <v>2448</v>
       </c>
@@ -1568,7 +1587,7 @@
         <v>0.1193939394</v>
       </c>
     </row>
-    <row r="35" spans="1:3" ht="204.75" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3" ht="192" x14ac:dyDescent="0.2">
       <c r="A35" s="3">
         <v>2495</v>
       </c>
@@ -1579,7 +1598,7 @@
         <v>0.1248617512</v>
       </c>
     </row>
-    <row r="36" spans="1:3" ht="78.75" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3" ht="64" x14ac:dyDescent="0.2">
       <c r="A36" s="3">
         <v>2439</v>
       </c>
@@ -1590,7 +1609,7 @@
         <v>0.125</v>
       </c>
     </row>
-    <row r="37" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:3" ht="32" x14ac:dyDescent="0.2">
       <c r="A37" s="3">
         <v>875</v>
       </c>
@@ -1601,7 +1620,7 @@
         <v>0.12656249999999999</v>
       </c>
     </row>
-    <row r="38" spans="1:3" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:3" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A38" s="3">
         <v>2611</v>
       </c>
@@ -1612,7 +1631,7 @@
         <v>0.1284863946</v>
       </c>
     </row>
-    <row r="39" spans="1:3" ht="110.25" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:3" ht="96" x14ac:dyDescent="0.2">
       <c r="A39" s="3">
         <v>1861</v>
       </c>
@@ -1623,7 +1642,7 @@
         <v>0.12946428569999999</v>
       </c>
     </row>
-    <row r="40" spans="1:3" ht="252" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:3" ht="224" x14ac:dyDescent="0.2">
       <c r="A40" s="3">
         <v>2321</v>
       </c>
@@ -1634,7 +1653,7 @@
         <v>0.13098958329999999</v>
       </c>
     </row>
-    <row r="41" spans="1:3" ht="204.75" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:3" ht="176" x14ac:dyDescent="0.2">
       <c r="A41" s="3">
         <v>2229</v>
       </c>
@@ -1645,7 +1664,7 @@
         <v>0.1315848214</v>
       </c>
     </row>
-    <row r="42" spans="1:3" ht="204.75" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:3" ht="176" x14ac:dyDescent="0.2">
       <c r="A42" s="3">
         <v>1561</v>
       </c>
@@ -1656,7 +1675,7 @@
         <v>0.13260368659999999</v>
       </c>
     </row>
-    <row r="43" spans="1:3" ht="220.5" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:3" ht="192" x14ac:dyDescent="0.2">
       <c r="A43" s="3">
         <v>247</v>
       </c>
@@ -1667,7 +1686,7 @@
         <v>0.13459183669999999</v>
       </c>
     </row>
-    <row r="44" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:3" ht="32" x14ac:dyDescent="0.2">
       <c r="A44" s="3">
         <v>49</v>
       </c>
@@ -1678,7 +1697,7 @@
         <v>0.13636363639999999</v>
       </c>
     </row>
-    <row r="45" spans="1:3" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:3" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A45" s="3">
         <v>2366</v>
       </c>
@@ -1689,7 +1708,7 @@
         <v>0.13948116560000001</v>
       </c>
     </row>
-    <row r="46" spans="1:3" ht="236.25" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:3" ht="208" x14ac:dyDescent="0.2">
       <c r="A46" s="3">
         <v>269</v>
       </c>
@@ -1700,7 +1719,7 @@
         <v>0.14343711840000001</v>
       </c>
     </row>
-    <row r="47" spans="1:3" ht="204.75" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:3" ht="192" x14ac:dyDescent="0.2">
       <c r="A47" s="3">
         <v>1941</v>
       </c>
@@ -1711,7 +1730,7 @@
         <v>0.14408482140000001</v>
       </c>
     </row>
-    <row r="48" spans="1:3" ht="252" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:3" ht="240" x14ac:dyDescent="0.2">
       <c r="A48" s="3">
         <v>268</v>
       </c>
@@ -1722,7 +1741,7 @@
         <v>0.1442307692</v>
       </c>
     </row>
-    <row r="49" spans="1:3" ht="204.75" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:3" ht="192" x14ac:dyDescent="0.2">
       <c r="A49" s="3">
         <v>2107</v>
       </c>
@@ -1733,7 +1752,7 @@
         <v>0.14682539680000001</v>
       </c>
     </row>
-    <row r="50" spans="1:3" ht="63" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:3" ht="64" x14ac:dyDescent="0.2">
       <c r="A50" s="3">
         <v>1603</v>
       </c>
@@ -1744,7 +1763,7 @@
         <v>0.1472222222</v>
       </c>
     </row>
-    <row r="51" spans="1:3" ht="220.5" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:3" ht="192" x14ac:dyDescent="0.2">
       <c r="A51" s="3">
         <v>91</v>
       </c>
@@ -1755,7 +1774,7 @@
         <v>0.148877551</v>
       </c>
     </row>
-    <row r="52" spans="1:3" ht="110.25" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:3" ht="96" x14ac:dyDescent="0.2">
       <c r="A52" s="3">
         <v>1690</v>
       </c>
@@ -1766,7 +1785,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="53" spans="1:3" ht="78.75" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:3" ht="80" x14ac:dyDescent="0.2">
       <c r="A53" s="3">
         <v>2757</v>
       </c>
@@ -1777,7 +1796,7 @@
         <v>0.15277777779999999</v>
       </c>
     </row>
-    <row r="54" spans="1:3" ht="220.5" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:3" ht="192" x14ac:dyDescent="0.2">
       <c r="A54" s="3">
         <v>2009</v>
       </c>
@@ -1788,7 +1807,7 @@
         <v>0.153877551</v>
       </c>
     </row>
-    <row r="55" spans="1:3" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:3" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A55" s="3">
         <v>2542</v>
       </c>
@@ -1799,7 +1818,7 @@
         <v>0.15770673809999999</v>
       </c>
     </row>
-    <row r="56" spans="1:3" ht="110.25" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:3" ht="112" x14ac:dyDescent="0.2">
       <c r="A56" s="3">
         <v>1302</v>
       </c>
@@ -1810,7 +1829,7 @@
         <v>0.1600649351</v>
       </c>
     </row>
-    <row r="57" spans="1:3" ht="220.5" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:3" ht="192" x14ac:dyDescent="0.2">
       <c r="A57" s="3">
         <v>607</v>
       </c>
@@ -1821,7 +1840,7 @@
         <v>0.16184210530000001</v>
       </c>
     </row>
-    <row r="58" spans="1:3" ht="189" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:3" ht="160" x14ac:dyDescent="0.2">
       <c r="A58" s="3">
         <v>1044</v>
       </c>
@@ -1832,7 +1851,7 @@
         <v>0.16450793650000001</v>
       </c>
     </row>
-    <row r="59" spans="1:3" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:3" ht="384" x14ac:dyDescent="0.2">
       <c r="A59" s="3">
         <v>2708</v>
       </c>
@@ -1843,7 +1862,7 @@
         <v>0.1645885547</v>
       </c>
     </row>
-    <row r="60" spans="1:3" ht="141.75" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:3" ht="128" x14ac:dyDescent="0.2">
       <c r="A60" s="3">
         <v>2801</v>
       </c>
@@ -1854,7 +1873,7 @@
         <v>0.16603174600000001</v>
       </c>
     </row>
-    <row r="61" spans="1:3" ht="141.75" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:3" ht="128" x14ac:dyDescent="0.2">
       <c r="A61" s="3">
         <v>2557</v>
       </c>
@@ -1865,7 +1884,7 @@
         <v>0.16666666669999999</v>
       </c>
     </row>
-    <row r="62" spans="1:3" ht="141.75" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:3" ht="128" x14ac:dyDescent="0.2">
       <c r="A62" s="3">
         <v>2519</v>
       </c>
@@ -1876,7 +1895,7 @@
         <v>0.16666666669999999</v>
       </c>
     </row>
-    <row r="63" spans="1:3" ht="141.75" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:3" ht="128" x14ac:dyDescent="0.2">
       <c r="A63" s="3">
         <v>1052</v>
       </c>
@@ -1887,7 +1906,7 @@
         <v>0.1875</v>
       </c>
     </row>
-    <row r="64" spans="1:3" ht="126" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:3" ht="112" x14ac:dyDescent="0.2">
       <c r="A64" s="3">
         <v>1747</v>
       </c>
@@ -1898,7 +1917,7 @@
         <v>0.18839285710000001</v>
       </c>
     </row>
-    <row r="65" spans="1:3" ht="189" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:3" ht="176" x14ac:dyDescent="0.2">
       <c r="A65" s="3">
         <v>2490</v>
       </c>
@@ -1909,7 +1928,7 @@
         <v>0.19223057639999999</v>
       </c>
     </row>
-    <row r="66" spans="1:3" ht="173.25" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:3" ht="144" x14ac:dyDescent="0.2">
       <c r="A66" s="3">
         <v>1278</v>
       </c>
@@ -1920,7 +1939,7 @@
         <v>0.19464285710000001</v>
       </c>
     </row>
-    <row r="67" spans="1:3" ht="157.5" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:3" ht="144" x14ac:dyDescent="0.2">
       <c r="A67" s="3">
         <v>1343</v>
       </c>
@@ -1931,7 +1950,7 @@
         <v>0.19464285710000001</v>
       </c>
     </row>
-    <row r="68" spans="1:3" ht="94.5" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:3" ht="96" x14ac:dyDescent="0.2">
       <c r="A68" s="3">
         <v>769</v>
       </c>
@@ -1942,7 +1961,7 @@
         <v>0.1964285714</v>
       </c>
     </row>
-    <row r="69" spans="1:3" ht="220.5" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:3" ht="208" x14ac:dyDescent="0.2">
       <c r="A69" s="3">
         <v>2696</v>
       </c>
@@ -1953,7 +1972,7 @@
         <v>0.1995098039</v>
       </c>
     </row>
-    <row r="70" spans="1:3" ht="220.5" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:3" ht="208" x14ac:dyDescent="0.2">
       <c r="A70" s="3">
         <v>1134</v>
       </c>
@@ -1964,7 +1983,7 @@
         <v>0.1995098039</v>
       </c>
     </row>
-    <row r="71" spans="1:3" ht="173.25" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:3" ht="160" x14ac:dyDescent="0.2">
       <c r="A71" s="3">
         <v>1327</v>
       </c>
@@ -1975,7 +1994,7 @@
         <v>0.20066844919999999</v>
       </c>
     </row>
-    <row r="72" spans="1:3" ht="189" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:3" ht="176" x14ac:dyDescent="0.2">
       <c r="A72" s="3">
         <v>1466</v>
       </c>
@@ -1986,7 +2005,7 @@
         <v>0.2041666667</v>
       </c>
     </row>
-    <row r="73" spans="1:3" ht="173.25" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:3" ht="160" x14ac:dyDescent="0.2">
       <c r="A73" s="3">
         <v>1211</v>
       </c>
@@ -1997,7 +2016,7 @@
         <v>0.20468749999999999</v>
       </c>
     </row>
-    <row r="74" spans="1:3" ht="63" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:3" ht="48" x14ac:dyDescent="0.2">
       <c r="A74" s="3">
         <v>806</v>
       </c>
@@ -2008,7 +2027,7 @@
         <v>0.20863095240000001</v>
       </c>
     </row>
-    <row r="75" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:3" ht="32" x14ac:dyDescent="0.2">
       <c r="A75" s="3">
         <v>921</v>
       </c>
@@ -2019,7 +2038,7 @@
         <v>0.22222222220000001</v>
       </c>
     </row>
-    <row r="76" spans="1:3" ht="126" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:3" ht="112" x14ac:dyDescent="0.2">
       <c r="A76" s="3">
         <v>2793</v>
       </c>
@@ -2030,7 +2049,7 @@
         <v>0.22797619050000001</v>
       </c>
     </row>
-    <row r="77" spans="1:3" ht="126" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:3" ht="112" x14ac:dyDescent="0.2">
       <c r="A77" s="3">
         <v>2159</v>
       </c>
@@ -2041,7 +2060,7 @@
         <v>0.23531144779999999</v>
       </c>
     </row>
-    <row r="78" spans="1:3" ht="126" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:3" ht="112" x14ac:dyDescent="0.2">
       <c r="A78" s="3">
         <v>2099</v>
       </c>
@@ -2052,7 +2071,7 @@
         <v>0.2666666667</v>
       </c>
     </row>
-    <row r="79" spans="1:3" ht="204.75" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:3" ht="176" x14ac:dyDescent="0.2">
       <c r="A79" s="3">
         <v>1186</v>
       </c>
@@ -2063,7 +2082,7 @@
         <v>0.27031250000000001</v>
       </c>
     </row>
-    <row r="80" spans="1:3" ht="94.5" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:3" ht="80" x14ac:dyDescent="0.2">
       <c r="A80" s="3">
         <v>690</v>
       </c>
@@ -2074,7 +2093,7 @@
         <v>0.27407407410000001</v>
       </c>
     </row>
-    <row r="81" spans="1:3" ht="63" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:3" ht="64" x14ac:dyDescent="0.2">
       <c r="A81" s="3">
         <v>1091</v>
       </c>
@@ -2085,7 +2104,7 @@
         <v>0.27500000000000002</v>
       </c>
     </row>
-    <row r="82" spans="1:3" ht="220.5" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:3" ht="192" x14ac:dyDescent="0.2">
       <c r="A82" s="3">
         <v>1490</v>
       </c>
@@ -2096,7 +2115,7 @@
         <v>0.27858974359999999</v>
       </c>
     </row>
-    <row r="83" spans="1:3" ht="63" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:3" ht="64" x14ac:dyDescent="0.2">
       <c r="A83" s="3">
         <v>1526</v>
       </c>
@@ -2107,7 +2126,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A84" s="3">
         <v>748</v>
       </c>
@@ -2118,7 +2137,7 @@
         <v>0.3111111111</v>
       </c>
     </row>
-    <row r="85" spans="1:3" ht="173.25" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:3" ht="160" x14ac:dyDescent="0.2">
       <c r="A85" s="3">
         <v>1295</v>
       </c>
@@ -2129,7 +2148,7 @@
         <v>0.32933333329999998</v>
       </c>
     </row>
-    <row r="86" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:3" ht="32" x14ac:dyDescent="0.2">
       <c r="A86" s="3">
         <v>411</v>
       </c>
@@ -2140,7 +2159,7 @@
         <v>0.3305555556</v>
       </c>
     </row>
-    <row r="87" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:3" ht="32" x14ac:dyDescent="0.2">
       <c r="A87" s="3">
         <v>2496</v>
       </c>
@@ -2151,7 +2170,7 @@
         <v>0.3305555556</v>
       </c>
     </row>
-    <row r="88" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:3" ht="48" x14ac:dyDescent="0.2">
       <c r="A88" s="3">
         <v>2747</v>
       </c>
@@ -2162,7 +2181,7 @@
         <v>0.35857142860000002</v>
       </c>
     </row>
-    <row r="89" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:3" ht="32" x14ac:dyDescent="0.2">
       <c r="A89" s="3">
         <v>958</v>
       </c>
@@ -2173,7 +2192,7 @@
         <v>0.38750000000000001</v>
       </c>
     </row>
-    <row r="90" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:3" ht="48" x14ac:dyDescent="0.2">
       <c r="A90" s="3">
         <v>880</v>
       </c>
@@ -2184,7 +2203,7 @@
         <v>0.39</v>
       </c>
     </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A91" s="3">
         <v>2427</v>
       </c>
@@ -2195,7 +2214,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A92" s="3">
         <v>927</v>
       </c>
@@ -2206,7 +2225,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="93" spans="1:3" ht="63" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:3" ht="64" x14ac:dyDescent="0.2">
       <c r="A93" s="3">
         <v>1105</v>
       </c>
@@ -2217,7 +2236,7 @@
         <v>0.60000000000000009</v>
       </c>
     </row>
-    <row r="94" spans="1:3" ht="78.75" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:3" ht="64" x14ac:dyDescent="0.2">
       <c r="A94" s="3">
         <v>1127</v>
       </c>
@@ -2228,7 +2247,7 @@
         <v>0.60000000000000009</v>
       </c>
     </row>
-    <row r="95" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:3" ht="32" x14ac:dyDescent="0.2">
       <c r="A95" s="3">
         <v>2302</v>
       </c>
@@ -2239,7 +2258,7 @@
         <v>0.61111111110000005</v>
       </c>
     </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A96" s="3">
         <v>2413</v>
       </c>
@@ -2258,21 +2277,22 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:C96"/>
+  <dimension ref="A1:D96"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="8.85546875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="136.140625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="15.5703125" style="1" customWidth="1"/>
-    <col min="4" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="8.83203125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="136.1640625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="15.5" style="1" customWidth="1"/>
+    <col min="4" max="4" width="14.5" style="1" customWidth="1"/>
+    <col min="5" max="16384" width="9.1640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="2"/>
       <c r="B1" s="3" t="s">
         <v>0</v>
@@ -2280,8 +2300,11 @@
       <c r="C1" s="3" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" ht="78.75" x14ac:dyDescent="0.25">
+      <c r="D1" s="5" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="64" x14ac:dyDescent="0.2">
       <c r="A2" s="3">
         <v>2841</v>
       </c>
@@ -2292,7 +2315,7 @@
         <v>-0.234375</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="63" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" ht="64" x14ac:dyDescent="0.2">
       <c r="A3" s="3">
         <v>2243</v>
       </c>
@@ -2303,7 +2326,7 @@
         <v>-8.7500000000000008E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="94.5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" ht="96" x14ac:dyDescent="0.2">
       <c r="A4" s="3">
         <v>1485</v>
       </c>
@@ -2314,7 +2337,7 @@
         <v>-8.1250000000000003E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="173.25" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" ht="144" x14ac:dyDescent="0.2">
       <c r="A5" s="3">
         <v>1429</v>
       </c>
@@ -2325,7 +2348,7 @@
         <v>-3.1278659600000001E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="157.5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" ht="144" x14ac:dyDescent="0.2">
       <c r="A6" s="3">
         <v>896</v>
       </c>
@@ -2336,7 +2359,7 @@
         <v>-2.9047619E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" ht="48" x14ac:dyDescent="0.2">
       <c r="A7" s="3">
         <v>595</v>
       </c>
@@ -2347,7 +2370,7 @@
         <v>-2.5000000000000001E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="3">
         <v>2210</v>
       </c>
@@ -2358,7 +2381,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" s="3">
         <v>2292</v>
       </c>
@@ -2369,7 +2392,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A10" s="3">
         <v>1251</v>
       </c>
@@ -2380,7 +2403,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" ht="48" x14ac:dyDescent="0.2">
       <c r="A11" s="3">
         <v>1734</v>
       </c>
@@ -2391,7 +2414,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" s="3">
         <v>20</v>
       </c>
@@ -2402,7 +2425,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="299.25" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" ht="272" x14ac:dyDescent="0.2">
       <c r="A13" s="3">
         <v>733</v>
       </c>
@@ -2413,7 +2436,7 @@
         <v>5.4421768999999998E-3</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="94.5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" ht="96" x14ac:dyDescent="0.2">
       <c r="A14" s="3">
         <v>651</v>
       </c>
@@ -2424,7 +2447,7 @@
         <v>1.38888889E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="78.75" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" ht="80" x14ac:dyDescent="0.2">
       <c r="A15" s="3">
         <v>1653</v>
       </c>
@@ -2435,7 +2458,7 @@
         <v>3.24675325E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="78.75" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" ht="80" x14ac:dyDescent="0.2">
       <c r="A16" s="3">
         <v>610</v>
       </c>
@@ -2446,7 +2469,7 @@
         <v>4.2063492100000002E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" ht="384" x14ac:dyDescent="0.2">
       <c r="A17" s="3">
         <v>1364</v>
       </c>
@@ -2457,7 +2480,7 @@
         <v>4.5686778499999997E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="110.25" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" ht="96" x14ac:dyDescent="0.2">
       <c r="A18" s="3">
         <v>2729</v>
       </c>
@@ -2468,7 +2491,7 @@
         <v>5.0264550300000002E-2</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" ht="48" x14ac:dyDescent="0.2">
       <c r="A19" s="3">
         <v>1210</v>
       </c>
@@ -2479,7 +2502,7 @@
         <v>5.4464285699999997E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A20" s="3">
         <v>1599</v>
       </c>
@@ -2490,7 +2513,7 @@
         <v>6.6023465200000006E-2</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="78.75" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" ht="64" x14ac:dyDescent="0.2">
       <c r="A21" s="3">
         <v>431</v>
       </c>
@@ -2501,7 +2524,7 @@
         <v>7.0000000000000007E-2</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="315" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" ht="272" x14ac:dyDescent="0.2">
       <c r="A22" s="3">
         <v>2434</v>
       </c>
@@ -2512,7 +2535,7 @@
         <v>7.0155341300000007E-2</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" ht="32" x14ac:dyDescent="0.2">
       <c r="A23" s="3">
         <v>1502</v>
       </c>
@@ -2523,7 +2546,7 @@
         <v>7.4999999999999997E-2</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="157.5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" ht="144" x14ac:dyDescent="0.2">
       <c r="A24" s="3">
         <v>1598</v>
       </c>
@@ -2534,7 +2557,7 @@
         <v>8.2043650800000006E-2</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A25" s="3">
         <v>2563</v>
       </c>
@@ -2545,7 +2568,7 @@
         <v>8.2783482700000008E-2</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" s="3">
         <v>908</v>
       </c>
@@ -2556,7 +2579,7 @@
         <v>8.3333333300000006E-2</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="189" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" ht="176" x14ac:dyDescent="0.2">
       <c r="A27" s="3">
         <v>440</v>
       </c>
@@ -2567,7 +2590,7 @@
         <v>8.8725490200000007E-2</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="94.5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" ht="96" x14ac:dyDescent="0.2">
       <c r="A28" s="3">
         <v>1381</v>
       </c>
@@ -2578,7 +2601,7 @@
         <v>9.0151515200000004E-2</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" ht="32" x14ac:dyDescent="0.2">
       <c r="A29" s="3">
         <v>2258</v>
       </c>
@@ -2589,7 +2612,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="220.5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" ht="192" x14ac:dyDescent="0.2">
       <c r="A30" s="3">
         <v>1918</v>
       </c>
@@ -2600,7 +2623,7 @@
         <v>0.1003061224</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="204.75" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" ht="176" x14ac:dyDescent="0.2">
       <c r="A31" s="3">
         <v>419</v>
       </c>
@@ -2611,7 +2634,7 @@
         <v>0.1021164021</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="126" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" ht="112" x14ac:dyDescent="0.2">
       <c r="A32" s="3">
         <v>1191</v>
       </c>
@@ -2622,7 +2645,7 @@
         <v>0.1063492063</v>
       </c>
     </row>
-    <row r="33" spans="1:3" ht="110.25" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" ht="96" x14ac:dyDescent="0.2">
       <c r="A33" s="3">
         <v>2730</v>
       </c>
@@ -2633,7 +2656,7 @@
         <v>0.1182539683</v>
       </c>
     </row>
-    <row r="34" spans="1:3" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A34" s="3">
         <v>2789</v>
       </c>
@@ -2644,7 +2667,7 @@
         <v>0.1193939394</v>
       </c>
     </row>
-    <row r="35" spans="1:3" ht="78.75" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3" ht="64" x14ac:dyDescent="0.2">
       <c r="A35" s="3">
         <v>883</v>
       </c>
@@ -2655,7 +2678,7 @@
         <v>0.1208333333</v>
       </c>
     </row>
-    <row r="36" spans="1:3" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A36" s="3">
         <v>2613</v>
       </c>
@@ -2666,7 +2689,7 @@
         <v>0.12253550539999999</v>
       </c>
     </row>
-    <row r="37" spans="1:3" ht="220.5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:3" ht="192" x14ac:dyDescent="0.2">
       <c r="A37" s="3">
         <v>191</v>
       </c>
@@ -2677,7 +2700,7 @@
         <v>0.12456709959999999</v>
       </c>
     </row>
-    <row r="38" spans="1:3" ht="204.75" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:3" ht="192" x14ac:dyDescent="0.2">
       <c r="A38" s="3">
         <v>1095</v>
       </c>
@@ -2688,7 +2711,7 @@
         <v>0.12462585029999999</v>
       </c>
     </row>
-    <row r="39" spans="1:3" ht="204.75" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:3" ht="192" x14ac:dyDescent="0.2">
       <c r="A39" s="3">
         <v>2495</v>
       </c>
@@ -2699,7 +2722,7 @@
         <v>0.1248617512</v>
       </c>
     </row>
-    <row r="40" spans="1:3" ht="189" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:3" ht="176" x14ac:dyDescent="0.2">
       <c r="A40" s="3">
         <v>2000</v>
       </c>
@@ -2710,7 +2733,7 @@
         <v>0.12488095239999999</v>
       </c>
     </row>
-    <row r="41" spans="1:3" ht="204.75" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:3" ht="192" x14ac:dyDescent="0.2">
       <c r="A41" s="3">
         <v>1943</v>
       </c>
@@ -2721,7 +2744,7 @@
         <v>0.12580532210000001</v>
       </c>
     </row>
-    <row r="42" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:3" ht="32" x14ac:dyDescent="0.2">
       <c r="A42" s="3">
         <v>875</v>
       </c>
@@ -2732,7 +2755,7 @@
         <v>0.12656249999999999</v>
       </c>
     </row>
-    <row r="43" spans="1:3" ht="220.5" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:3" ht="192" x14ac:dyDescent="0.2">
       <c r="A43" s="3">
         <v>1938</v>
       </c>
@@ -2743,7 +2766,7 @@
         <v>0.12845982140000001</v>
       </c>
     </row>
-    <row r="44" spans="1:3" ht="204.75" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:3" ht="176" x14ac:dyDescent="0.2">
       <c r="A44" s="3">
         <v>2151</v>
       </c>
@@ -2754,7 +2777,7 @@
         <v>0.12845982140000001</v>
       </c>
     </row>
-    <row r="45" spans="1:3" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:3" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A45" s="3">
         <v>2605</v>
       </c>
@@ -2765,7 +2788,7 @@
         <v>0.1284863946</v>
       </c>
     </row>
-    <row r="46" spans="1:3" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:3" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A46" s="3">
         <v>2609</v>
       </c>
@@ -2776,7 +2799,7 @@
         <v>0.1284863946</v>
       </c>
     </row>
-    <row r="47" spans="1:3" ht="220.5" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:3" ht="192" x14ac:dyDescent="0.2">
       <c r="A47" s="3">
         <v>1915</v>
       </c>
@@ -2787,7 +2810,7 @@
         <v>0.13260368659999999</v>
       </c>
     </row>
-    <row r="48" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:3" ht="32" x14ac:dyDescent="0.2">
       <c r="A48" s="3">
         <v>1716</v>
       </c>
@@ -2798,7 +2821,7 @@
         <v>0.1333333333</v>
       </c>
     </row>
-    <row r="49" spans="1:3" ht="204.75" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:3" ht="176" x14ac:dyDescent="0.2">
       <c r="A49" s="3">
         <v>14</v>
       </c>
@@ -2809,7 +2832,7 @@
         <v>0.13627232140000001</v>
       </c>
     </row>
-    <row r="50" spans="1:3" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:3" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A50" s="3">
         <v>2503</v>
       </c>
@@ -2820,7 +2843,7 @@
         <v>0.13948116560000001</v>
       </c>
     </row>
-    <row r="51" spans="1:3" ht="236.25" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:3" ht="224" x14ac:dyDescent="0.2">
       <c r="A51" s="3">
         <v>2488</v>
       </c>
@@ -2831,7 +2854,7 @@
         <v>0.1406746032</v>
       </c>
     </row>
-    <row r="52" spans="1:3" ht="236.25" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:3" ht="224" x14ac:dyDescent="0.2">
       <c r="A52" s="3">
         <v>2567</v>
       </c>
@@ -2842,7 +2865,7 @@
         <v>0.14236559139999999</v>
       </c>
     </row>
-    <row r="53" spans="1:3" ht="94.5" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:3" ht="80" x14ac:dyDescent="0.2">
       <c r="A53" s="3">
         <v>79</v>
       </c>
@@ -2853,7 +2876,7 @@
         <v>0.14259259260000001</v>
       </c>
     </row>
-    <row r="54" spans="1:3" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:3" ht="400" x14ac:dyDescent="0.2">
       <c r="A54" s="3">
         <v>2101</v>
       </c>
@@ -2864,7 +2887,7 @@
         <v>0.14426877469999999</v>
       </c>
     </row>
-    <row r="55" spans="1:3" ht="236.25" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:3" ht="224" x14ac:dyDescent="0.2">
       <c r="A55" s="3">
         <v>1988</v>
       </c>
@@ -2875,7 +2898,7 @@
         <v>0.1457521645</v>
       </c>
     </row>
-    <row r="56" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:3" ht="48" x14ac:dyDescent="0.2">
       <c r="A56" s="3">
         <v>383</v>
       </c>
@@ -2886,7 +2909,7 @@
         <v>0.1466666667</v>
       </c>
     </row>
-    <row r="57" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:3" ht="48" x14ac:dyDescent="0.2">
       <c r="A57" s="3">
         <v>1839</v>
       </c>
@@ -2897,7 +2920,7 @@
         <v>0.14687500000000001</v>
       </c>
     </row>
-    <row r="58" spans="1:3" ht="220.5" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:3" ht="192" x14ac:dyDescent="0.2">
       <c r="A58" s="3">
         <v>1917</v>
       </c>
@@ -2908,7 +2931,7 @@
         <v>0.146877551</v>
       </c>
     </row>
-    <row r="59" spans="1:3" ht="63" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:3" ht="48" x14ac:dyDescent="0.2">
       <c r="A59" s="3">
         <v>8</v>
       </c>
@@ -2919,7 +2942,7 @@
         <v>0.15476190479999999</v>
       </c>
     </row>
-    <row r="60" spans="1:3" ht="220.5" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:3" ht="192" x14ac:dyDescent="0.2">
       <c r="A60" s="3">
         <v>372</v>
       </c>
@@ -2930,7 +2953,7 @@
         <v>0.1552536232</v>
       </c>
     </row>
-    <row r="61" spans="1:3" ht="157.5" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:3" ht="144" x14ac:dyDescent="0.2">
       <c r="A61" s="3">
         <v>1810</v>
       </c>
@@ -2941,7 +2964,7 @@
         <v>0.15588235289999999</v>
       </c>
     </row>
-    <row r="62" spans="1:3" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:3" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A62" s="3">
         <v>1382</v>
       </c>
@@ -2952,7 +2975,7 @@
         <v>0.1621609403</v>
       </c>
     </row>
-    <row r="63" spans="1:3" ht="78.75" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:3" ht="80" x14ac:dyDescent="0.2">
       <c r="A63" s="3">
         <v>2192</v>
       </c>
@@ -2963,7 +2986,7 @@
         <v>0.16567460319999999</v>
       </c>
     </row>
-    <row r="64" spans="1:3" ht="141.75" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:3" ht="128" x14ac:dyDescent="0.2">
       <c r="A64" s="3">
         <v>513</v>
       </c>
@@ -2974,7 +2997,7 @@
         <v>0.16666666669999999</v>
       </c>
     </row>
-    <row r="65" spans="1:3" ht="63" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:3" ht="64" x14ac:dyDescent="0.2">
       <c r="A65" s="3">
         <v>1411</v>
       </c>
@@ -2985,7 +3008,7 @@
         <v>0.16742424240000001</v>
       </c>
     </row>
-    <row r="66" spans="1:3" ht="252" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:3" ht="224" x14ac:dyDescent="0.2">
       <c r="A66" s="3">
         <v>1840</v>
       </c>
@@ -2996,7 +3019,7 @@
         <v>0.17780612239999999</v>
       </c>
     </row>
-    <row r="67" spans="1:3" ht="78.75" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:3" ht="64" x14ac:dyDescent="0.2">
       <c r="A67" s="3">
         <v>32</v>
       </c>
@@ -3007,7 +3030,7 @@
         <v>0.18333333330000001</v>
       </c>
     </row>
-    <row r="68" spans="1:3" ht="173.25" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:3" ht="144" x14ac:dyDescent="0.2">
       <c r="A68" s="3">
         <v>706</v>
       </c>
@@ -3018,7 +3041,7 @@
         <v>0.185</v>
       </c>
     </row>
-    <row r="69" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:3" ht="32" x14ac:dyDescent="0.2">
       <c r="A69" s="3">
         <v>836</v>
       </c>
@@ -3029,7 +3052,7 @@
         <v>0.1875</v>
       </c>
     </row>
-    <row r="70" spans="1:3" ht="252" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:3" ht="224" x14ac:dyDescent="0.2">
       <c r="A70" s="3">
         <v>2115</v>
       </c>
@@ -3040,7 +3063,7 @@
         <v>0.1922193878</v>
       </c>
     </row>
-    <row r="71" spans="1:3" ht="189" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:3" ht="176" x14ac:dyDescent="0.2">
       <c r="A71" s="3">
         <v>2490</v>
       </c>
@@ -3051,7 +3074,7 @@
         <v>0.19223057639999999</v>
       </c>
     </row>
-    <row r="72" spans="1:3" ht="220.5" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:3" ht="208" x14ac:dyDescent="0.2">
       <c r="A72" s="3">
         <v>2652</v>
       </c>
@@ -3062,7 +3085,7 @@
         <v>0.1995098039</v>
       </c>
     </row>
-    <row r="73" spans="1:3" ht="220.5" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:3" ht="208" x14ac:dyDescent="0.2">
       <c r="A73" s="3">
         <v>2710</v>
       </c>
@@ -3073,7 +3096,7 @@
         <v>0.1995098039</v>
       </c>
     </row>
-    <row r="74" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A74" s="3">
         <v>494</v>
       </c>
@@ -3084,7 +3107,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="75" spans="1:3" ht="63" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:3" ht="64" x14ac:dyDescent="0.2">
       <c r="A75" s="3">
         <v>2194</v>
       </c>
@@ -3095,7 +3118,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="76" spans="1:3" ht="236.25" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:3" ht="208" x14ac:dyDescent="0.2">
       <c r="A76" s="3">
         <v>1111</v>
       </c>
@@ -3106,7 +3129,7 @@
         <v>0.20340909090000001</v>
       </c>
     </row>
-    <row r="77" spans="1:3" ht="110.25" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:3" ht="96" x14ac:dyDescent="0.2">
       <c r="A77" s="3">
         <v>451</v>
       </c>
@@ -3117,7 +3140,7 @@
         <v>0.21047619049999999</v>
       </c>
     </row>
-    <row r="78" spans="1:3" ht="173.25" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:3" ht="144" x14ac:dyDescent="0.2">
       <c r="A78" s="3">
         <v>1223</v>
       </c>
@@ -3128,7 +3151,7 @@
         <v>0.215</v>
       </c>
     </row>
-    <row r="79" spans="1:3" ht="94.5" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:3" ht="80" x14ac:dyDescent="0.2">
       <c r="A79" s="3">
         <v>685</v>
       </c>
@@ -3139,7 +3162,7 @@
         <v>0.21689393940000001</v>
       </c>
     </row>
-    <row r="80" spans="1:3" ht="189" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:3" ht="176" x14ac:dyDescent="0.2">
       <c r="A80" s="3">
         <v>2493</v>
       </c>
@@ -3150,7 +3173,7 @@
         <v>0.21931818180000001</v>
       </c>
     </row>
-    <row r="81" spans="1:3" ht="110.25" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:3" ht="96" x14ac:dyDescent="0.2">
       <c r="A81" s="3">
         <v>385</v>
       </c>
@@ -3161,7 +3184,7 @@
         <v>0.2211038961</v>
       </c>
     </row>
-    <row r="82" spans="1:3" ht="126" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:3" ht="112" x14ac:dyDescent="0.2">
       <c r="A82" s="3">
         <v>1172</v>
       </c>
@@ -3172,7 +3195,7 @@
         <v>0.2273809524</v>
       </c>
     </row>
-    <row r="83" spans="1:3" ht="220.5" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:3" ht="192" x14ac:dyDescent="0.2">
       <c r="A83" s="3">
         <v>1491</v>
       </c>
@@ -3183,7 +3206,7 @@
         <v>0.22747294370000001</v>
       </c>
     </row>
-    <row r="84" spans="1:3" ht="204.75" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:3" ht="176" x14ac:dyDescent="0.2">
       <c r="A84" s="3">
         <v>708</v>
       </c>
@@ -3194,7 +3217,7 @@
         <v>0.23375000000000001</v>
       </c>
     </row>
-    <row r="85" spans="1:3" ht="141.75" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:3" ht="128" x14ac:dyDescent="0.2">
       <c r="A85" s="3">
         <v>863</v>
       </c>
@@ -3205,7 +3228,7 @@
         <v>0.2354081633</v>
       </c>
     </row>
-    <row r="86" spans="1:3" ht="78.75" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:3" ht="80" x14ac:dyDescent="0.2">
       <c r="A86" s="3">
         <v>1035</v>
       </c>
@@ -3216,7 +3239,7 @@
         <v>0.23749999999999999</v>
       </c>
     </row>
-    <row r="87" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:3" ht="48" x14ac:dyDescent="0.2">
       <c r="A87" s="3">
         <v>761</v>
       </c>
@@ -3227,7 +3250,7 @@
         <v>0.23749999999999999</v>
       </c>
     </row>
-    <row r="88" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:3" ht="32" x14ac:dyDescent="0.2">
       <c r="A88" s="3">
         <v>2796</v>
       </c>
@@ -3238,7 +3261,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="89" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:3" ht="32" x14ac:dyDescent="0.2">
       <c r="A89" s="3">
         <v>1021</v>
       </c>
@@ -3249,7 +3272,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="90" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:3" ht="32" x14ac:dyDescent="0.2">
       <c r="A90" s="3">
         <v>886</v>
       </c>
@@ -3260,7 +3283,7 @@
         <v>0.2666666667</v>
       </c>
     </row>
-    <row r="91" spans="1:3" ht="126" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:3" ht="112" x14ac:dyDescent="0.2">
       <c r="A91" s="3">
         <v>1914</v>
       </c>
@@ -3271,7 +3294,7 @@
         <v>0.27307692309999998</v>
       </c>
     </row>
-    <row r="92" spans="1:3" ht="78.75" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:3" ht="64" x14ac:dyDescent="0.2">
       <c r="A92" s="3">
         <v>2731</v>
       </c>
@@ -3282,7 +3305,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="93" spans="1:3" ht="126" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:3" ht="112" x14ac:dyDescent="0.2">
       <c r="A93" s="3">
         <v>2102</v>
       </c>
@@ -3293,7 +3316,7 @@
         <v>0.34230769230000002</v>
       </c>
     </row>
-    <row r="94" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:3" ht="48" x14ac:dyDescent="0.2">
       <c r="A94" s="3">
         <v>2254</v>
       </c>
@@ -3304,7 +3327,7 @@
         <v>0.38789682539999998</v>
       </c>
     </row>
-    <row r="95" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:3" ht="32" x14ac:dyDescent="0.2">
       <c r="A95" s="3">
         <v>714</v>
       </c>
@@ -3315,7 +3338,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="96" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A96" s="3">
         <v>866</v>
       </c>
@@ -3333,21 +3356,21 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:C96"/>
+  <dimension ref="A1:D96"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="8.85546875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="136.140625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="15.5703125" style="1" customWidth="1"/>
-    <col min="4" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="8.83203125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="136.1640625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="15.5" style="1" customWidth="1"/>
+    <col min="4" max="16384" width="9.1640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="2"/>
       <c r="B1" s="3" t="s">
         <v>0</v>
@@ -3355,8 +3378,11 @@
       <c r="C1" s="3" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="D1" s="5" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A2" s="3">
         <v>585</v>
       </c>
@@ -3367,7 +3393,7 @@
         <v>-0.10625</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A3" s="3">
         <v>847</v>
       </c>
@@ -3378,7 +3404,7 @@
         <v>-9.5000000000000001E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="63" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" ht="64" x14ac:dyDescent="0.2">
       <c r="A4" s="3">
         <v>1546</v>
       </c>
@@ -3389,18 +3415,18 @@
         <v>-7.7499999999999999E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" ht="48" x14ac:dyDescent="0.2">
       <c r="A5" s="3">
         <v>181</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="4" t="s">
         <v>186</v>
       </c>
       <c r="C5" s="2">
         <v>-7.1428571400000002E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="3">
         <v>965</v>
       </c>
@@ -3411,7 +3437,7 @@
         <v>-6.25E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="63" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" ht="48" x14ac:dyDescent="0.2">
       <c r="A7" s="3">
         <v>1773</v>
       </c>
@@ -3422,7 +3448,7 @@
         <v>-0.05</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A8" s="3">
         <v>2688</v>
       </c>
@@ -3433,7 +3459,7 @@
         <v>-3.3333333299999997E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="126" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" ht="112" x14ac:dyDescent="0.2">
       <c r="A9" s="3">
         <v>2343</v>
       </c>
@@ -3444,7 +3470,7 @@
         <v>-1.64021164E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="126" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" ht="112" x14ac:dyDescent="0.2">
       <c r="A10" s="3">
         <v>935</v>
       </c>
@@ -3455,7 +3481,7 @@
         <v>-8.0952381000000007E-3</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" s="3">
         <v>2441</v>
       </c>
@@ -3466,7 +3492,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" s="3">
         <v>1202</v>
       </c>
@@ -3477,7 +3503,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" s="3">
         <v>1265</v>
       </c>
@@ -3488,7 +3514,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" ht="48" x14ac:dyDescent="0.2">
       <c r="A14" s="3">
         <v>1695</v>
       </c>
@@ -3499,7 +3525,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" s="3">
         <v>1259</v>
       </c>
@@ -3510,7 +3536,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" s="3">
         <v>1192</v>
       </c>
@@ -3521,7 +3547,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" s="3">
         <v>2223</v>
       </c>
@@ -3532,7 +3558,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="110.25" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" ht="96" x14ac:dyDescent="0.2">
       <c r="A18" s="3">
         <v>632</v>
       </c>
@@ -3543,7 +3569,7 @@
         <v>1.0416666999999999E-3</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="141.75" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" ht="128" x14ac:dyDescent="0.2">
       <c r="A19" s="3">
         <v>1048</v>
       </c>
@@ -3554,7 +3580,7 @@
         <v>9.1666667000000011E-3</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="252" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" ht="224" x14ac:dyDescent="0.2">
       <c r="A20" s="3">
         <v>200</v>
       </c>
@@ -3565,7 +3591,7 @@
         <v>1.01851852E-2</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="283.5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" ht="256" x14ac:dyDescent="0.2">
       <c r="A21" s="3">
         <v>2247</v>
       </c>
@@ -3576,7 +3602,7 @@
         <v>2.3384353699999999E-2</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" ht="48" x14ac:dyDescent="0.2">
       <c r="A22" s="3">
         <v>2797</v>
       </c>
@@ -3587,7 +3613,7 @@
         <v>2.5000000000000001E-2</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="173.25" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" ht="160" x14ac:dyDescent="0.2">
       <c r="A23" s="3">
         <v>1376</v>
       </c>
@@ -3598,7 +3624,7 @@
         <v>2.6666666700000001E-2</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="141.75" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" ht="128" x14ac:dyDescent="0.2">
       <c r="A24" s="3">
         <v>1234</v>
       </c>
@@ -3609,7 +3635,7 @@
         <v>4.5238095200000002E-2</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="94.5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" ht="80" x14ac:dyDescent="0.2">
       <c r="A25" s="3">
         <v>360</v>
       </c>
@@ -3620,7 +3646,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" ht="32" x14ac:dyDescent="0.2">
       <c r="A26" s="3">
         <v>810</v>
       </c>
@@ -3631,7 +3657,7 @@
         <v>5.1666666700000002E-2</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" ht="368" x14ac:dyDescent="0.2">
       <c r="A27" s="3">
         <v>2723</v>
       </c>
@@ -3642,7 +3668,7 @@
         <v>6.41666667E-2</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="94.5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" ht="80" x14ac:dyDescent="0.2">
       <c r="A28" s="3">
         <v>2212</v>
       </c>
@@ -3653,7 +3679,7 @@
         <v>6.5000000000000002E-2</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" ht="32" x14ac:dyDescent="0.2">
       <c r="A29" s="3">
         <v>2133</v>
       </c>
@@ -3664,7 +3690,7 @@
         <v>6.6666666700000002E-2</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="378" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" ht="336" x14ac:dyDescent="0.2">
       <c r="A30" s="3">
         <v>1846</v>
       </c>
@@ -3675,7 +3701,7 @@
         <v>6.8055555599999998E-2</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="94.5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" ht="80" x14ac:dyDescent="0.2">
       <c r="A31" s="3">
         <v>44</v>
       </c>
@@ -3686,7 +3712,7 @@
         <v>6.8181818200000008E-2</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="78.75" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" ht="80" x14ac:dyDescent="0.2">
       <c r="A32" s="3">
         <v>17</v>
       </c>
@@ -3697,7 +3723,7 @@
         <v>7.0000000000000007E-2</v>
       </c>
     </row>
-    <row r="33" spans="1:3" ht="78.75" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" ht="64" x14ac:dyDescent="0.2">
       <c r="A33" s="3">
         <v>504</v>
       </c>
@@ -3708,7 +3734,7 @@
         <v>7.0000000000000007E-2</v>
       </c>
     </row>
-    <row r="34" spans="1:3" ht="78.75" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3" ht="64" x14ac:dyDescent="0.2">
       <c r="A34" s="3">
         <v>338</v>
       </c>
@@ -3719,7 +3745,7 @@
         <v>7.0000000000000007E-2</v>
       </c>
     </row>
-    <row r="35" spans="1:3" ht="78.75" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3" ht="64" x14ac:dyDescent="0.2">
       <c r="A35" s="3">
         <v>2642</v>
       </c>
@@ -3730,7 +3756,7 @@
         <v>7.0000000000000007E-2</v>
       </c>
     </row>
-    <row r="36" spans="1:3" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A36" s="3">
         <v>1385</v>
       </c>
@@ -3741,7 +3767,7 @@
         <v>9.1264480800000006E-2</v>
       </c>
     </row>
-    <row r="37" spans="1:3" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:3" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A37" s="3">
         <v>1591</v>
       </c>
@@ -3752,7 +3778,7 @@
         <v>9.1690831700000003E-2</v>
       </c>
     </row>
-    <row r="38" spans="1:3" ht="252" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:3" ht="224" x14ac:dyDescent="0.2">
       <c r="A38" s="3">
         <v>2418</v>
       </c>
@@ -3763,7 +3789,7 @@
         <v>9.8051948100000008E-2</v>
       </c>
     </row>
-    <row r="39" spans="1:3" ht="78.75" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:3" ht="80" x14ac:dyDescent="0.2">
       <c r="A39" s="3">
         <v>482</v>
       </c>
@@ -3774,7 +3800,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="40" spans="1:3" ht="94.5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:3" ht="80" x14ac:dyDescent="0.2">
       <c r="A40" s="3">
         <v>177</v>
       </c>
@@ -3785,7 +3811,7 @@
         <v>0.11273148149999999</v>
       </c>
     </row>
-    <row r="41" spans="1:3" ht="141.75" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:3" ht="128" x14ac:dyDescent="0.2">
       <c r="A41" s="3">
         <v>1568</v>
       </c>
@@ -3796,7 +3822,7 @@
         <v>0.1129166667</v>
       </c>
     </row>
-    <row r="42" spans="1:3" ht="346.5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:3" ht="320" x14ac:dyDescent="0.2">
       <c r="A42" s="3">
         <v>1797</v>
       </c>
@@ -3807,7 +3833,7 @@
         <v>0.11428571429999999</v>
       </c>
     </row>
-    <row r="43" spans="1:3" ht="189" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:3" ht="160" x14ac:dyDescent="0.2">
       <c r="A43" s="3">
         <v>1551</v>
       </c>
@@ -3818,7 +3844,7 @@
         <v>0.11521164020000001</v>
       </c>
     </row>
-    <row r="44" spans="1:3" ht="204.75" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:3" ht="176" x14ac:dyDescent="0.2">
       <c r="A44" s="3">
         <v>1931</v>
       </c>
@@ -3829,7 +3855,7 @@
         <v>0.11547619050000001</v>
       </c>
     </row>
-    <row r="45" spans="1:3" ht="110.25" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:3" ht="96" x14ac:dyDescent="0.2">
       <c r="A45" s="3">
         <v>2588</v>
       </c>
@@ -3840,7 +3866,7 @@
         <v>0.1182539683</v>
       </c>
     </row>
-    <row r="46" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:3" ht="48" x14ac:dyDescent="0.2">
       <c r="A46" s="3">
         <v>1022</v>
       </c>
@@ -3851,7 +3877,7 @@
         <v>0.11874999999999999</v>
       </c>
     </row>
-    <row r="47" spans="1:3" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:3" ht="368" x14ac:dyDescent="0.2">
       <c r="A47" s="3">
         <v>1017</v>
       </c>
@@ -3862,7 +3888,7 @@
         <v>0.1232453416</v>
       </c>
     </row>
-    <row r="48" spans="1:3" ht="94.5" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:3" ht="80" x14ac:dyDescent="0.2">
       <c r="A48" s="3">
         <v>477</v>
       </c>
@@ -3873,7 +3899,7 @@
         <v>0.12666666670000001</v>
       </c>
     </row>
-    <row r="49" spans="1:3" ht="220.5" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:3" ht="192" x14ac:dyDescent="0.2">
       <c r="A49" s="3">
         <v>2573</v>
       </c>
@@ -3884,7 +3910,7 @@
         <v>0.1276544402</v>
       </c>
     </row>
-    <row r="50" spans="1:3" ht="189" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:3" ht="176" x14ac:dyDescent="0.2">
       <c r="A50" s="3">
         <v>2706</v>
       </c>
@@ -3895,7 +3921,7 @@
         <v>0.12845982140000001</v>
       </c>
     </row>
-    <row r="51" spans="1:3" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:3" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A51" s="3">
         <v>2601</v>
       </c>
@@ -3906,7 +3932,7 @@
         <v>0.1284863946</v>
       </c>
     </row>
-    <row r="52" spans="1:3" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:3" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A52" s="3">
         <v>2608</v>
       </c>
@@ -3917,7 +3943,7 @@
         <v>0.1284863946</v>
       </c>
     </row>
-    <row r="53" spans="1:3" ht="267.75" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:3" ht="240" x14ac:dyDescent="0.2">
       <c r="A53" s="3">
         <v>266</v>
       </c>
@@ -3928,7 +3954,7 @@
         <v>0.13062499999999999</v>
       </c>
     </row>
-    <row r="54" spans="1:3" ht="220.5" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:3" ht="192" x14ac:dyDescent="0.2">
       <c r="A54" s="3">
         <v>491</v>
       </c>
@@ -3939,7 +3965,7 @@
         <v>0.1306277056</v>
       </c>
     </row>
-    <row r="55" spans="1:3" ht="204.75" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:3" ht="176" x14ac:dyDescent="0.2">
       <c r="A55" s="3">
         <v>3</v>
       </c>
@@ -3950,7 +3976,7 @@
         <v>0.13260368659999999</v>
       </c>
     </row>
-    <row r="56" spans="1:3" ht="204.75" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:3" ht="176" x14ac:dyDescent="0.2">
       <c r="A56" s="3">
         <v>1958</v>
       </c>
@@ -3961,7 +3987,7 @@
         <v>0.13260368659999999</v>
       </c>
     </row>
-    <row r="57" spans="1:3" ht="204.75" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:3" ht="176" x14ac:dyDescent="0.2">
       <c r="A57" s="3">
         <v>2651</v>
       </c>
@@ -3972,7 +3998,7 @@
         <v>0.13260368659999999</v>
       </c>
     </row>
-    <row r="58" spans="1:3" ht="204.75" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:3" ht="176" x14ac:dyDescent="0.2">
       <c r="A58" s="3">
         <v>14</v>
       </c>
@@ -3983,7 +4009,7 @@
         <v>0.13627232140000001</v>
       </c>
     </row>
-    <row r="59" spans="1:3" ht="220.5" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:3" ht="192" x14ac:dyDescent="0.2">
       <c r="A59" s="3">
         <v>2064</v>
       </c>
@@ -3994,7 +4020,7 @@
         <v>0.1385504202</v>
       </c>
     </row>
-    <row r="60" spans="1:3" ht="204.75" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:3" ht="176" x14ac:dyDescent="0.2">
       <c r="A60" s="3">
         <v>2066</v>
       </c>
@@ -4005,7 +4031,7 @@
         <v>0.14335637479999999</v>
       </c>
     </row>
-    <row r="61" spans="1:3" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:3" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A61" s="3">
         <v>2477</v>
       </c>
@@ -4016,7 +4042,7 @@
         <v>0.14725424279999999</v>
       </c>
     </row>
-    <row r="62" spans="1:3" ht="330.75" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:3" ht="288" x14ac:dyDescent="0.2">
       <c r="A62" s="3">
         <v>740</v>
       </c>
@@ -4027,7 +4053,7 @@
         <v>0.1560606061</v>
       </c>
     </row>
-    <row r="63" spans="1:3" ht="110.25" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:3" ht="96" x14ac:dyDescent="0.2">
       <c r="A63" s="3">
         <v>455</v>
       </c>
@@ -4038,7 +4064,7 @@
         <v>0.17499999999999999</v>
       </c>
     </row>
-    <row r="64" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:3" ht="48" x14ac:dyDescent="0.2">
       <c r="A64" s="3">
         <v>920</v>
       </c>
@@ -4049,7 +4075,7 @@
         <v>0.18</v>
       </c>
     </row>
-    <row r="65" spans="1:3" ht="267.75" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:3" ht="224" x14ac:dyDescent="0.2">
       <c r="A65" s="3">
         <v>2026</v>
       </c>
@@ -4060,7 +4086,7 @@
         <v>0.18035119050000001</v>
       </c>
     </row>
-    <row r="66" spans="1:3" ht="173.25" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:3" ht="144" x14ac:dyDescent="0.2">
       <c r="A66" s="3">
         <v>833</v>
       </c>
@@ -4071,7 +4097,7 @@
         <v>0.1840555556</v>
       </c>
     </row>
-    <row r="67" spans="1:3" ht="126" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:3" ht="112" x14ac:dyDescent="0.2">
       <c r="A67" s="3">
         <v>1747</v>
       </c>
@@ -4082,7 +4108,7 @@
         <v>0.18839285710000001</v>
       </c>
     </row>
-    <row r="68" spans="1:3" ht="157.5" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:3" ht="144" x14ac:dyDescent="0.2">
       <c r="A68" s="3">
         <v>284</v>
       </c>
@@ -4093,7 +4119,7 @@
         <v>0.19210758380000001</v>
       </c>
     </row>
-    <row r="69" spans="1:3" ht="157.5" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:3" ht="144" x14ac:dyDescent="0.2">
       <c r="A69" s="3">
         <v>278</v>
       </c>
@@ -4104,7 +4130,7 @@
         <v>0.19210758380000001</v>
       </c>
     </row>
-    <row r="70" spans="1:3" ht="157.5" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:3" ht="144" x14ac:dyDescent="0.2">
       <c r="A70" s="3">
         <v>317</v>
       </c>
@@ -4115,7 +4141,7 @@
         <v>0.19210758380000001</v>
       </c>
     </row>
-    <row r="71" spans="1:3" ht="157.5" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:3" ht="144" x14ac:dyDescent="0.2">
       <c r="A71" s="3">
         <v>1159</v>
       </c>
@@ -4126,7 +4152,7 @@
         <v>0.19464285710000001</v>
       </c>
     </row>
-    <row r="72" spans="1:3" ht="220.5" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:3" ht="208" x14ac:dyDescent="0.2">
       <c r="A72" s="3">
         <v>1144</v>
       </c>
@@ -4137,7 +4163,7 @@
         <v>0.1995098039</v>
       </c>
     </row>
-    <row r="73" spans="1:3" ht="78.75" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:3" ht="80" x14ac:dyDescent="0.2">
       <c r="A73" s="3">
         <v>2388</v>
       </c>
@@ -4148,7 +4174,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="74" spans="1:3" ht="252" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:3" ht="224" x14ac:dyDescent="0.2">
       <c r="A74" s="3">
         <v>7</v>
       </c>
@@ -4159,7 +4185,7 @@
         <v>0.2041806723</v>
       </c>
     </row>
-    <row r="75" spans="1:3" ht="126" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:3" ht="112" x14ac:dyDescent="0.2">
       <c r="A75" s="3">
         <v>105</v>
       </c>
@@ -4170,7 +4196,7 @@
         <v>0.22619047619999999</v>
       </c>
     </row>
-    <row r="76" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:3" ht="48" x14ac:dyDescent="0.2">
       <c r="A76" s="3">
         <v>966</v>
       </c>
@@ -4181,7 +4207,7 @@
         <v>0.23095238100000001</v>
       </c>
     </row>
-    <row r="77" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A77" s="3">
         <v>973</v>
       </c>
@@ -4192,7 +4218,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="78" spans="1:3" ht="173.25" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:3" ht="144" x14ac:dyDescent="0.2">
       <c r="A78" s="3">
         <v>1324</v>
       </c>
@@ -4203,7 +4229,7 @@
         <v>0.26386800329999999</v>
       </c>
     </row>
-    <row r="79" spans="1:3" ht="315" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:3" ht="272" x14ac:dyDescent="0.2">
       <c r="A79" s="3">
         <v>1097</v>
       </c>
@@ -4214,7 +4240,7 @@
         <v>0.26696428570000003</v>
       </c>
     </row>
-    <row r="80" spans="1:3" ht="126" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:3" ht="112" x14ac:dyDescent="0.2">
       <c r="A80" s="3">
         <v>2623</v>
       </c>
@@ -4225,7 +4251,7 @@
         <v>0.27307692309999998</v>
       </c>
     </row>
-    <row r="81" spans="1:3" ht="126" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:3" ht="112" x14ac:dyDescent="0.2">
       <c r="A81" s="3">
         <v>2616</v>
       </c>
@@ -4236,7 +4262,7 @@
         <v>0.27307692309999998</v>
       </c>
     </row>
-    <row r="82" spans="1:3" ht="126" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:3" ht="112" x14ac:dyDescent="0.2">
       <c r="A82" s="3">
         <v>294</v>
       </c>
@@ -4247,7 +4273,7 @@
         <v>0.27307692309999998</v>
       </c>
     </row>
-    <row r="83" spans="1:3" ht="94.5" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:3" ht="80" x14ac:dyDescent="0.2">
       <c r="A83" s="3">
         <v>690</v>
       </c>
@@ -4258,7 +4284,7 @@
         <v>0.27407407410000001</v>
       </c>
     </row>
-    <row r="84" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:3" ht="32" x14ac:dyDescent="0.2">
       <c r="A84" s="3">
         <v>1230</v>
       </c>
@@ -4269,7 +4295,7 @@
         <v>0.28333333329999999</v>
       </c>
     </row>
-    <row r="85" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:3" ht="32" x14ac:dyDescent="0.2">
       <c r="A85" s="3">
         <v>459</v>
       </c>
@@ -4280,7 +4306,7 @@
         <v>0.29375000000000001</v>
       </c>
     </row>
-    <row r="86" spans="1:3" ht="63" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:3" ht="64" x14ac:dyDescent="0.2">
       <c r="A86" s="3">
         <v>1526</v>
       </c>
@@ -4291,7 +4317,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="87" spans="1:3" ht="63" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:3" ht="64" x14ac:dyDescent="0.2">
       <c r="A87" s="3">
         <v>756</v>
       </c>
@@ -4302,7 +4328,7 @@
         <v>0.32500000000000001</v>
       </c>
     </row>
-    <row r="88" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:3" ht="32" x14ac:dyDescent="0.2">
       <c r="A88" s="3">
         <v>254</v>
       </c>
@@ -4313,7 +4339,7 @@
         <v>0.35</v>
       </c>
     </row>
-    <row r="89" spans="1:3" ht="189" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:3" ht="160" x14ac:dyDescent="0.2">
       <c r="A89" s="3">
         <v>2741</v>
       </c>
@@ -4324,7 +4350,7 @@
         <v>0.35754385960000001</v>
       </c>
     </row>
-    <row r="90" spans="1:3" ht="78.75" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:3" ht="64" x14ac:dyDescent="0.2">
       <c r="A90" s="3">
         <v>1523</v>
       </c>
@@ -4335,7 +4361,7 @@
         <v>0.36666666669999998</v>
       </c>
     </row>
-    <row r="91" spans="1:3" ht="393.75" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:3" ht="352" x14ac:dyDescent="0.2">
       <c r="A91" s="3">
         <v>2825</v>
       </c>
@@ -4346,7 +4372,7 @@
         <v>0.38742424240000001</v>
       </c>
     </row>
-    <row r="92" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:3" ht="48" x14ac:dyDescent="0.2">
       <c r="A92" s="3">
         <v>880</v>
       </c>
@@ -4357,7 +4383,7 @@
         <v>0.39</v>
       </c>
     </row>
-    <row r="93" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A93" s="3">
         <v>241</v>
       </c>
@@ -4368,7 +4394,7 @@
         <v>0.4114285714</v>
       </c>
     </row>
-    <row r="94" spans="1:3" ht="63" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:3" ht="48" x14ac:dyDescent="0.2">
       <c r="A94" s="3">
         <v>2134</v>
       </c>
@@ -4379,7 +4405,7 @@
         <v>0.4795918367</v>
       </c>
     </row>
-    <row r="95" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A95" s="3">
         <v>860</v>
       </c>
@@ -4390,7 +4416,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="96" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:3" ht="32" x14ac:dyDescent="0.2">
       <c r="A96" s="3">
         <v>2809</v>
       </c>
@@ -4404,4 +4430,16 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8930CA54-47A8-8845-98EB-5BACD4EE4291}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>